<commit_message>
Excels completed + additional comments
</commit_message>
<xml_diff>
--- a/excel/results_QLearning.xlsx
+++ b/excel/results_QLearning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ensuque\Documents\1-TRUE DOCUMENTS\Polytech\4A\ISI3\TP1\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AE2746-549F-4E45-9195-00FB44642C5B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{12C30767-B02C-4103-ABE2-3DD0B26E82AB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{227635A9-40B6-4196-97DE-A258BE6D7277}"/>
   </bookViews>
@@ -31,55 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t xml:space="preserve"> = 1 (Biais)</t>
-  </si>
-  <si>
-    <t>Nombre de fantômes qui peuvent atteindre en un pas la future position du pacman.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> =  1 si il y a un pacDot sur la prochaine position du pacman, 0 sinon.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> = </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dist(s,a) / mapsize</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, avec dist(s,a) la distance du pacman future avec le plus proche pacDot.</t>
-    </r>
-  </si>
-  <si>
-    <t>Distance fantôme le plus proche sur la nouvelle position.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> dist(s,a) / (mapX + mapY)</t>
-  </si>
-  <si>
-    <t>Notes:</t>
-  </si>
-  <si>
     <t>Critères choisis</t>
   </si>
   <si>
@@ -93,21 +49,6 @@
   </si>
   <si>
     <t>Nombre de Dots restant</t>
-  </si>
-  <si>
-    <t>Distance fantome le plus proche</t>
-  </si>
-  <si>
-    <t>Coordonnées Pacman</t>
-  </si>
-  <si>
-    <t>Direction du Dot le plus proche</t>
-  </si>
-  <si>
-    <t>Direction de déplacement valide du dot le plus proche</t>
-  </si>
-  <si>
-    <t>On regarde ici uniquement les cases vers lesquels le pacman peut se déplacer</t>
   </si>
   <si>
     <r>
@@ -210,11 +151,6 @@
 - Direction fantôme le plus proche (si d&lt;4)</t>
   </si>
   <si>
-    <t xml:space="preserve"> - Coordonnées Pacman
-- Distance fantôme le plus proche (si d&lt;4)
-- Direction fantôme le plus proche (si d&lt;4)</t>
-  </si>
-  <si>
     <t>65%
 (~180 Etats)</t>
   </si>
@@ -231,42 +167,10 @@
 (~140 Etats)</t>
   </si>
   <si>
-    <t>92%
-(~63 Etats)</t>
-  </si>
-  <si>
     <t>90%
 (~54 Etats)</t>
   </si>
   <si>
-    <t>93%
-(~135 Etats)</t>
-  </si>
-  <si>
-    <t>&lt;5%
-(~80 Etats)</t>
-  </si>
-  <si>
-    <t>&lt;5%
-(~1 200+ Etats)</t>
-  </si>
-  <si>
-    <t>&lt;5%
-(~300 Etats)</t>
-  </si>
-  <si>
-    <t>&lt;5%
-(~11 000+ Etats)</t>
-  </si>
-  <si>
-    <t>&lt;5%
-(~17 000+ Etats)</t>
-  </si>
-  <si>
-    <t>&lt;5%
-(~1 800+ Etats)</t>
-  </si>
-  <si>
     <t>90%
 (~100 Etats)</t>
   </si>
@@ -275,17 +179,232 @@
 (~150 Etats)</t>
   </si>
   <si>
-    <t>Distance fantome le plus proche (si d &lt;= 3 )</t>
-  </si>
-  <si>
-    <t>Si d &gt; 3, on utilisera une valeur par défaut pour éviter de multiplier les états.</t>
+    <t>90%
+(~63 Etats)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Direction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> fantôme le plus proche</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Distance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> fantome le plus proche (si d &lt;= 3 )</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Distance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> fantome le plus proche</t>
+    </r>
+  </si>
+  <si>
+    <t>Si le fantôme est à une distance &gt; 3 du Pacman, renvoie la valeur par défaut DIRECTION.STOP</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Direction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> fantôme le plus proche (si d &lt;= 3)</t>
+    </r>
+  </si>
+  <si>
+    <t>Renvoie la direction du fantôme le plus proche (NORTH, EAST, ect..)</t>
+  </si>
+  <si>
+    <t>Génère un hash à partir des coordonnées de chaque fantômes.</t>
+  </si>
+  <si>
+    <t>Distance de Manhattan.</t>
+  </si>
+  <si>
+    <t>Si le fantôme est à une distance &gt; 3 du Pacman, renvoie la valeur par défaut 0.</t>
+  </si>
+  <si>
+    <t>TROP LONG
+(~17 000+ Etats)</t>
+  </si>
+  <si>
+    <t>TROP LONG
+(~11 000+ Etats)</t>
+  </si>
+  <si>
+    <t>TROP LONG
+(~1 800+ Etats)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Direction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> valide du Dot le plus proche</t>
+    </r>
+  </si>
+  <si>
+    <t>(NORTH, EAST, ect..)
+On regarde ici uniquement les cases vers lesquels le pacman peut se déplacer</t>
+  </si>
+  <si>
+    <t>2%
+(~300 Etats)</t>
+  </si>
+  <si>
+    <t>50%
+(~25 Etats)</t>
+  </si>
+  <si>
+    <t>84%
+(~25 Etats)</t>
+  </si>
+  <si>
+    <t>97%
+(~25 Etats)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Direction Dot le plus proche
+- Direction fantôme le plus proche</t>
+  </si>
+  <si>
+    <t>81%
+(~166 Etats)</t>
+  </si>
+  <si>
+    <t>88%
+(~37 Etats)</t>
+  </si>
+  <si>
+    <t>95%
+(~36 Etats)</t>
+  </si>
+  <si>
+    <t>68%
+(~20 Etats)</t>
+  </si>
+  <si>
+    <t>3%
+(~20 Etats)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Direction Dot le plus proche
+- Direction fantôme le plus proche (d &lt; 4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Direction Dot le plus proche
+- Direction fantôme le plus proche (d &lt; 4)
+- Distance fantôme  le plus proche</t>
+  </si>
+  <si>
+    <t>16%
+(~20 Etats)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Direction Dot le plus proche
+- Distance Dot le plus proche
+- Distance fantôme  le plus proche (d &lt; 4)
+- Direction fantôme  le plus proche (d &lt; 4)</t>
+  </si>
+  <si>
+    <t>90%
+(~118 Etats)</t>
+  </si>
+  <si>
+    <t>90%
+(~161 Etats)</t>
+  </si>
+  <si>
+    <t>40%
+(~1200+ Etats)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,16 +420,85 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -327,11 +515,163 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -339,15 +679,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -360,9 +691,90 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="5" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Insatisfaisant" xfId="2" builtinId="27"/>
+    <cellStyle name="Neutre" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -674,18 +1086,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E22599B-B8A4-49E2-8DD2-C6B6769DF984}">
-  <dimension ref="B3:N30"/>
+  <dimension ref="B3:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="50.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1"/>
+    <col min="4" max="4" width="39.85546875" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
@@ -700,9 +1112,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -711,17 +1121,17 @@
     </row>
     <row r="4" spans="2:14" ht="45" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="29" t="s">
         <v>8</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="2"/>
@@ -730,17 +1140,17 @@
     </row>
     <row r="5" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
-      <c r="D5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>36</v>
+      <c r="D5" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="J5" s="1"/>
       <c r="M5" s="1"/>
@@ -748,17 +1158,17 @@
     </row>
     <row r="6" spans="2:14" ht="45" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
-      <c r="D6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>37</v>
+      <c r="D6" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="J6" s="1"/>
       <c r="M6" s="1"/>
@@ -766,57 +1176,57 @@
     </row>
     <row r="7" spans="2:14" ht="45" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
-      <c r="D7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="D7" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
       <c r="J7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="2:14" ht="45" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
-      <c r="D8" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="6" t="s">
+      <c r="D8" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
       <c r="J8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="2:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
-      <c r="D9" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>34</v>
+      <c r="D9" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -824,24 +1234,40 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="D10" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>47</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" ht="45" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="D11" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>40</v>
+      </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="1"/>
@@ -850,12 +1276,20 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" ht="60" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+      <c r="D12" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>51</v>
+      </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="1"/>
@@ -866,10 +1300,10 @@
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="1"/>
@@ -880,10 +1314,10 @@
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="1"/>
@@ -894,10 +1328,10 @@
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="1"/>
@@ -907,16 +1341,16 @@
       <c r="N15" s="1"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="B16" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -925,17 +1359,17 @@
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
     </row>
-    <row r="17" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
+    <row r="17" spans="2:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="B17" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -944,17 +1378,16 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
     </row>
-    <row r="18" spans="2:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
+    <row r="18" spans="2:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -963,14 +1396,11 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
     </row>
-    <row r="19" spans="2:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="9"/>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="21"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -981,12 +1411,12 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
     </row>
-    <row r="20" spans="2:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>4</v>
+    <row r="20" spans="2:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>28</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -999,11 +1429,11 @@
       <c r="N20" s="1"/>
     </row>
     <row r="21" spans="2:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>42</v>
+      <c r="B21" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>29</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1016,12 +1446,13 @@
       <c r="N21" s="1"/>
     </row>
     <row r="22" spans="2:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="B22" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1032,11 +1463,13 @@
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
     </row>
-    <row r="23" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="1"/>
+    <row r="23" spans="2:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="B23" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>24</v>
+      </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -1048,15 +1481,12 @@
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
     </row>
-    <row r="24" spans="2:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" t="s">
-        <v>6</v>
+    <row r="24" spans="2:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="B24" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>34</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1070,7 +1500,8 @@
       <c r="N24" s="1"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C25" s="1"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -1084,9 +1515,7 @@
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="D26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1104,9 +1533,6 @@
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D30" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>